<commit_message>
Refactor scheduler model and improve code formatting
Added detailed comments and improved code formatting for clarity in the SchedulerModel and related modules. Enhanced variable naming and line breaks for readability, especially in constraint and indicator construction. Updated schedule output files to reflect new session assignments and fixed minor logic issues in the Excel writer and time utilities.
</commit_message>
<xml_diff>
--- a/output/schedule.xlsx
+++ b/output/schedule.xlsx
@@ -7,10 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="R1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="R2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Therapists" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Patients" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="R2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Therapists" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Patients" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,11 +424,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="34" customWidth="1" min="4" max="4"/>
-    <col width="34" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="43" customWidth="1" min="2" max="2"/>
+    <col width="41" customWidth="1" min="3" max="3"/>
+    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="41" customWidth="1" min="5" max="5"/>
+    <col width="43" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -484,6 +483,16 @@
           <t>10:00-11:00</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>occupational_therapy | P2 | T2 | R2 | n=1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>occupational_therapy | P2 | T2 | R2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -505,6 +514,11 @@
           <t>14:00-15:00</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>kinesiology | P1 | T3 | R2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -519,6 +533,21 @@
           <t>16:00-17:00</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>phonoaudiology | P1, P3 | T1 | R2 | n=2</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>phonoaudiology | P1, P3 | T1 | R2 | n=2</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -528,12 +557,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>kinesiology | P1 | T3 | R1 | n=1</t>
+          <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>kinesiology | P1 | T3 | R1 | n=1</t>
+          <t>kinesiology | P1 | T3 | R2 | n=1</t>
         </is>
       </c>
     </row>
@@ -548,7 +577,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,49 +585,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="43" customWidth="1" min="2" max="2"/>
-    <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="37" customWidth="1" min="4" max="4"/>
-    <col width="37" customWidth="1" min="5" max="5"/>
-    <col width="43" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="41" customWidth="1" min="3" max="3"/>
+    <col width="43" customWidth="1" min="4" max="4"/>
+    <col width="34" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Friday</t>
+          <t>T3</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>08:00-09:00</t>
         </is>
       </c>
@@ -606,6 +634,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>09:00-10:00</t>
         </is>
       </c>
@@ -613,15 +646,15 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>10:00-11:00</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>occupational_therapy | P2 | T2 | R2 | n=1</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>occupational_therapy | P2 | T2 | R2 | n=1</t>
         </is>
@@ -630,6 +663,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>11:00-12:00</t>
         </is>
       </c>
@@ -637,6 +675,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>12:00-13:00</t>
         </is>
       </c>
@@ -644,39 +687,39 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>14:00-15:00</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>15:00-16:00</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P3 | T1 | R2 | n=1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>16:00-17:00</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
         </is>
@@ -685,17 +728,474 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>phonoaudiology | P1, P3 | T1 | R2 | n=2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>kinesiology | P1 | T3 | R2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
         <is>
           <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P3 | T1 | R2 | n=1</t>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>phonoaudiology | P1, P3 | T1 | R2 | n=2</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>kinesiology | P1 | T3 | R2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>occupational_therapy | P2 | T2 | R2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
         </is>
       </c>
     </row>
@@ -720,9 +1220,9 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="37" customWidth="1" min="3" max="3"/>
+    <col width="41" customWidth="1" min="3" max="3"/>
     <col width="43" customWidth="1" min="4" max="4"/>
-    <col width="34" customWidth="1" min="5" max="5"/>
+    <col width="41" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -738,17 +1238,17 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>P3</t>
         </is>
       </c>
     </row>
@@ -953,11 +1453,6 @@
           <t>15:00-16:00</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P3 | T1 | R2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -970,6 +1465,16 @@
           <t>16:00-17:00</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>phonoaudiology | P1, P3 | T1 | R2 | n=2</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>phonoaudiology | P1, P3 | T1 | R2 | n=2</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -982,11 +1487,6 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1061,7 +1561,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
+          <t>kinesiology | P1 | T3 | R2 | n=1</t>
         </is>
       </c>
     </row>
@@ -1100,9 +1600,9 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>kinesiology | P1 | T3 | R1 | n=1</t>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
         </is>
       </c>
     </row>
@@ -1177,11 +1677,6 @@
           <t>14:00-15:00</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1206,6 +1701,16 @@
           <t>16:00-17:00</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>phonoaudiology | P1, P3 | T1 | R2 | n=2</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>phonoaudiology | P1, P3 | T1 | R2 | n=2</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1220,655 +1725,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>phonoaudiology | P3 | T1 | R2 | n=1</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>kinesiology | P1 | T3 | R1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>occupational_therapy | P2 | T2 | R2 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E46"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="43" customWidth="1" min="4" max="4"/>
-    <col width="37" customWidth="1" min="5" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Day</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>P1</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>P2</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>P3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>occupational_therapy | P2 | T2 | R2 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P3 | T1 | R2 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>kinesiology | P1 | T3 | R1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P1 | T1 | R2 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>kinesiology | P1 | T3 | R1 | n=1</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>phonoaudiology | P3 | T1 | R2 | n=1</t>
+          <t>kinesiology | P1 | T3 | R2 | n=1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor model to use therapies instead of specialties
Replaces specialty-based scheduling with therapy-based logic across API, data loader, and Excel writer. Updates data schemas, validation, and sample data to define therapies with required specialties and patient bounds, and adjusts patient, room, and session structures to reference therapies. Improves schedule output format and validation to match new therapy-centric model.
</commit_message>
<xml_diff>
--- a/output/schedule.xlsx
+++ b/output/schedule.xlsx
@@ -7,11 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="4" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="R1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="sala colegio" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Therapists" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Patients" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="s1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="s2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Therapists" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Patients" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,11 +425,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="35" customWidth="1" min="2" max="2"/>
-    <col width="35" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="35" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="36" customWidth="1" min="4" max="4"/>
+    <col width="36" customWidth="1" min="5" max="5"/>
+    <col width="39" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -478,14 +477,9 @@
           <t>09:00-10:00</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 3 | T1 | 4 | n=1</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 4 | T1 | 4 | n=1</t>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
         </is>
       </c>
     </row>
@@ -495,6 +489,11 @@
           <t>10:00-11:00</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>kine_1 | joseto | kine:mau | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -502,14 +501,9 @@
           <t>11:00-12:00</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 7 | T1 | 4 | n=1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 4 | T1 | 4 | n=1</t>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:mau | s1 | n=1</t>
         </is>
       </c>
     </row>
@@ -519,6 +513,16 @@
           <t>12:00-13:00</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>kine_1 | joseto | kine:maca | s1 | n=1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:mau | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -538,11 +542,6 @@
       <c r="A9" t="inlineStr">
         <is>
           <t>16:00-17:00</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 4 | T1 | 4 | n=1</t>
         </is>
       </c>
     </row>
@@ -574,10 +573,10 @@
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="39" customWidth="1" min="2" max="2"/>
-    <col width="36" customWidth="1" min="3" max="3"/>
-    <col width="36" customWidth="1" min="4" max="4"/>
-    <col width="32" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="58" customWidth="1" min="3" max="3"/>
+    <col width="39" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="39" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -618,9 +617,9 @@
           <t>08:00-09:00</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>kinesiology | 7 | T1 | R1 | n=1</t>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:mau | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -630,11 +629,6 @@
           <t>09:00-10:00</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>kinesiology | 2 | 4 | R1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -642,6 +636,11 @@
           <t>10:00-11:00</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:mau | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -656,11 +655,6 @@
           <t>12:00-13:00</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>kinesiology | 3 | 2 | R1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -668,14 +662,9 @@
           <t>14:00-15:00</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>paes grupal | 2, 3, 4 | T1 | R1 | n=3</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>kinesiology | 4 | 2 | R1 | n=1</t>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:mau | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -685,14 +674,19 @@
           <t>15:00-16:00</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>kinesiology | 4 | 4 | R1 | n=1</t>
-        </is>
-      </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>phonoaudiology | 7 | T1 | R1 | n=1</t>
+          <t>tea_group | agu, joseto | fono:javi, kine:mau | s2 | n=2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:mau | s2 | n=1</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:mau | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -702,26 +696,11 @@
           <t>16:00-17:00</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>kinesiology | 2 | 4 | R1 | n=1</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 7 | T1 | R1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
           <t>17:00-18:00</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>kinesiology | 4 | 4 | R1 | n=1</t>
         </is>
       </c>
     </row>
@@ -736,7 +715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -744,49 +723,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="56" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="58" customWidth="1" min="3" max="3"/>
+    <col width="40" customWidth="1" min="4" max="4"/>
+    <col width="58" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>javi</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>maca</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Friday</t>
+          <t>mau</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>08:00-09:00</t>
         </is>
       </c>
@@ -794,6 +772,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>09:00-10:00</t>
         </is>
       </c>
@@ -801,30 +784,40 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>10:00-11:00</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>visita colegio | 2 | visitadora 1 | sala colegio | n=1</t>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:mau | s2 | n=1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>11:00-12:00</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>visita colegio | 2 | visitadora 1 | sala colegio | n=1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>12:00-13:00</t>
         </is>
       </c>
@@ -832,6 +825,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>14:00-15:00</t>
         </is>
       </c>
@@ -839,24 +837,521 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>15:00-16:00</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>visita colegio | 2 | visitadora 1 | sala colegio | n=1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>16:00-17:00</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:mau | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>kine_1 | joseto | kine:maca | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:mau | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>tea_group | agu, joseto | fono:javi, kine:mau | s2 | n=2</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>tea_group | agu, joseto | fono:javi, kine:mau | s2 | n=2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:mau | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:mau | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:mau | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>kine_1 | joseto | kine:mau | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:mau | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
         <is>
           <t>17:00-18:00</t>
         </is>
@@ -873,7 +1368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -883,10 +1378,8 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="32" customWidth="1" min="3" max="3"/>
-    <col width="32" customWidth="1" min="4" max="4"/>
-    <col width="39" customWidth="1" min="5" max="5"/>
-    <col width="56" customWidth="1" min="6" max="6"/>
+    <col width="58" customWidth="1" min="3" max="3"/>
+    <col width="58" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -902,22 +1395,12 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>agu</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>visitadora 1</t>
+          <t>joseto</t>
         </is>
       </c>
     </row>
@@ -932,11 +1415,6 @@
           <t>08:00-09:00</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>kinesiology | 7 | T1 | R1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -949,16 +1427,6 @@
           <t>09:00-10:00</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>kinesiology | 2 | 4 | R1 | n=1</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 3 | T1 | 4 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -971,9 +1439,9 @@
           <t>10:00-11:00</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>visita colegio | 2 | visitadora 1 | sala colegio | n=1</t>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:mau | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -988,16 +1456,6 @@
           <t>11:00-12:00</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 7 | T1 | 4 | n=1</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>visita colegio | 2 | visitadora 1 | sala colegio | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1010,11 +1468,6 @@
           <t>12:00-13:00</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>kinesiology | 3 | 2 | R1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1027,11 +1480,6 @@
           <t>14:00-15:00</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>paes grupal | 2, 3, 4 | T1 | R1 | n=3</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1044,16 +1492,6 @@
           <t>15:00-16:00</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>kinesiology | 4 | 4 | R1 | n=1</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>visita colegio | 2 | visitadora 1 | sala colegio | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1066,16 +1504,6 @@
           <t>16:00-17:00</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>kinesiology | 2 | 4 | R1 | n=1</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 4 | T1 | 4 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1100,6 +1528,11 @@
           <t>08:00-09:00</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:mau | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1112,6 +1545,11 @@
           <t>09:00-10:00</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1136,11 +1574,6 @@
           <t>11:00-12:00</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 4 | T1 | 4 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1153,6 +1586,11 @@
           <t>12:00-13:00</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>kine_1 | joseto | kine:maca | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1165,6 +1603,11 @@
           <t>14:00-15:00</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:mau | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1177,9 +1620,14 @@
           <t>15:00-16:00</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 7 | T1 | R1 | n=1</t>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>tea_group | agu, joseto | fono:javi, kine:mau | s2 | n=2</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>tea_group | agu, joseto | fono:javi, kine:mau | s2 | n=2</t>
         </is>
       </c>
     </row>
@@ -1206,11 +1654,6 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>kinesiology | 4 | 4 | R1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1271,6 +1714,11 @@
           <t>12:00-13:00</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:mau | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1295,6 +1743,11 @@
           <t>15:00-16:00</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:mau | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1307,11 +1760,6 @@
           <t>16:00-17:00</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 7 | T1 | R1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1348,11 +1796,6 @@
           <t>09:00-10:00</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 4 | T1 | 4 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1377,6 +1820,11 @@
           <t>11:00-12:00</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:mau | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1401,11 +1849,6 @@
           <t>14:00-15:00</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>kinesiology | 4 | 2 | R1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1478,6 +1921,11 @@
           <t>10:00-11:00</t>
         </is>
       </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>kine_1 | joseto | kine:mau | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1526,703 +1974,9 @@
           <t>15:00-16:00</t>
         </is>
       </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F46"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="56" customWidth="1" min="3" max="3"/>
-    <col width="39" customWidth="1" min="4" max="4"/>
-    <col width="39" customWidth="1" min="5" max="5"/>
-    <col width="36" customWidth="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Day</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>kinesiology | 7 | T1 | R1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>kinesiology | 2 | 4 | R1 | n=1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 3 | T1 | 4 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>visita colegio | 2 | visitadora 1 | sala colegio | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>visita colegio | 2 | visitadora 1 | sala colegio | n=1</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 7 | T1 | 4 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>kinesiology | 3 | 2 | R1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>paes grupal | 2, 3, 4 | T1 | R1 | n=3</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>paes grupal | 2, 3, 4 | T1 | R1 | n=3</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>paes grupal | 2, 3, 4 | T1 | R1 | n=3</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>visita colegio | 2 | visitadora 1 | sala colegio | n=1</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>kinesiology | 4 | 4 | R1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>kinesiology | 2 | 4 | R1 | n=1</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 4 | T1 | 4 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 4 | T1 | 4 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 7 | T1 | R1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>kinesiology | 4 | 4 | R1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 7 | T1 | R1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>phonoaudiology | 4 | T1 | 4 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>kinesiology | 4 | 2 | R1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:mau | s2 | n=1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve entity tables and scheduling logic
Removed availability columns from entity tables and added scroll area for better UI usability. Updated therapist and patient data, improved schedule generation to include new sessions, and refined diagnostics display logic. Enhanced scroll bar styling for consistency.
</commit_message>
<xml_diff>
--- a/output/schedule.xlsx
+++ b/output/schedule.xlsx
@@ -7,8 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Therapists" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Patients" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="s1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="s2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Therapists" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Patients" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,30 +424,49 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="37" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="37" customWidth="1" min="5" max="5"/>
+    <col width="52" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Day</t>
+          <t>Time</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Time</t>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Friday</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
           <t>08:00-09:00</t>
         </is>
       </c>
@@ -453,23 +474,18 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
           <t>09:00-10:00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:7 | s1 | n=1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
           <t>10:00-11:00</t>
         </is>
       </c>
@@ -477,11 +493,6 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
           <t>11:00-12:00</t>
         </is>
       </c>
@@ -489,23 +500,18 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>12:00-13:00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>12:00-13:00</t>
+          <t>kine_1 | joseto | kine:7 | s1 | n=1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
           <t>14:00-15:00</t>
         </is>
       </c>
@@ -513,468 +519,41 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
           <t>15:00-16:00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:7 | s1 | n=1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>16:00-17:00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16:00-17:00</t>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>taller_2 | agu, joseto | fono:5, kine:7 | s1 | n=2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
           <t>17:00-18:00</t>
         </is>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>kine_1 | joseto | kine:7 | s1 | n=1</t>
         </is>
       </c>
     </row>
@@ -989,7 +568,159 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="53" customWidth="1" min="2" max="2"/>
+    <col width="37" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="37" customWidth="1" min="5" max="5"/>
+    <col width="37" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:7 | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>tea_group | agu, joseto | fono:5, kine:7 | s2 | n=2</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -999,6 +730,9 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="53" customWidth="1" min="3" max="3"/>
+    <col width="53" customWidth="1" min="4" max="4"/>
+    <col width="37" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1012,6 +746,21 @@
           <t>Time</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>javi</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1072,6 +821,11 @@
           <t>12:00-13:00</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>kine_1 | joseto | kine:7 | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1084,6 +838,11 @@
           <t>14:00-15:00</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1108,6 +867,11 @@
           <t>16:00-17:00</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1120,6 +884,16 @@
           <t>17:00-18:00</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>tea_group | agu, joseto | fono:5, kine:7 | s2 | n=2</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>tea_group | agu, joseto | fono:5, kine:7 | s2 | n=2</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1144,6 +918,11 @@
           <t>09:00-10:00</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1348,6 +1127,11 @@
           <t>08:00-09:00</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1420,6 +1204,11 @@
           <t>15:00-16:00</t>
         </is>
       </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:7 | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1444,6 +1233,11 @@
           <t>17:00-18:00</t>
         </is>
       </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>kine_1 | joseto | kine:7 | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1456,6 +1250,11 @@
           <t>08:00-09:00</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1468,6 +1267,11 @@
           <t>09:00-10:00</t>
         </is>
       </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:7 | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1504,6 +1308,11 @@
           <t>12:00-13:00</t>
         </is>
       </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:7 | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1538,6 +1347,673 @@
       <c r="B45" t="inlineStr">
         <is>
           <t>16:00-17:00</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>taller_2 | agu, joseto | fono:5, kine:7 | s1 | n=2</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>taller_2 | agu, joseto | fono:5, kine:7 | s1 | n=2</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="53" customWidth="1" min="3" max="3"/>
+    <col width="53" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>agu</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>joseto</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>kine_1 | joseto | kine:7 | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>tea_group | agu, joseto | fono:5, kine:7 | s2 | n=2</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>tea_group | agu, joseto | fono:5, kine:7 | s2 | n=2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:7 | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>kine_1 | joseto | kine:7 | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:7 | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:7 | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>taller_2 | agu, joseto | fono:5, kine:7 | s1 | n=2</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>taller_2 | agu, joseto | fono:5, kine:7 | s1 | n=2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add support for fixed therapists per patient and therapy
Introduces the ability to specify fixed therapists for each patient and therapy, including validation and UI for assignment. Updates data models, API payloads, backend validation, and the UI to allow users to assign specific therapists to therapy specialties for patients. Adjusts scheduling logic to enforce these constraints and updates schema validation accordingly.
</commit_message>
<xml_diff>
--- a/output/schedule.xlsx
+++ b/output/schedule.xlsx
@@ -426,10 +426,10 @@
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="37" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="37" customWidth="1" min="5" max="5"/>
-    <col width="52" customWidth="1" min="6" max="6"/>
+    <col width="37" customWidth="1" min="3" max="3"/>
+    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -477,11 +477,6 @@
           <t>09:00-10:00</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:7 | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -489,6 +484,11 @@
           <t>10:00-11:00</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -503,11 +503,6 @@
           <t>12:00-13:00</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>kine_1 | joseto | kine:7 | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -522,9 +517,9 @@
           <t>15:00-16:00</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:7 | s1 | n=1</t>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
         </is>
       </c>
     </row>
@@ -534,16 +529,6 @@
           <t>16:00-17:00</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>taller_2 | agu, joseto | fono:5, kine:7 | s1 | n=2</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -551,9 +536,9 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>kine_1 | joseto | kine:7 | s1 | n=1</t>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
         </is>
       </c>
     </row>
@@ -577,11 +562,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="53" customWidth="1" min="2" max="2"/>
+    <col width="37" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="37" customWidth="1" min="5" max="5"/>
-    <col width="37" customWidth="1" min="6" max="6"/>
+    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -622,14 +607,9 @@
           <t>08:00-09:00</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -639,11 +619,6 @@
           <t>09:00-10:00</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -665,11 +640,6 @@
           <t>12:00-13:00</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:7 | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -679,7 +649,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -701,11 +676,6 @@
       <c r="A10" t="inlineStr">
         <is>
           <t>17:00-18:00</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>tea_group | agu, joseto | fono:5, kine:7 | s2 | n=2</t>
         </is>
       </c>
     </row>
@@ -715,669 +685,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E46"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="53" customWidth="1" min="3" max="3"/>
-    <col width="53" customWidth="1" min="4" max="4"/>
-    <col width="37" customWidth="1" min="5" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Day</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>javi</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>kine_1 | joseto | kine:7 | s1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>tea_group | agu, joseto | fono:5, kine:7 | s2 | n=2</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>tea_group | agu, joseto | fono:5, kine:7 | s2 | n=2</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:7 | s1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>kine_1 | joseto | kine:7 | s1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>08:00-09:00</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>09:00-10:00</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:7 | s1 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>10:00-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>11:00-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>12:00-13:00</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:7 | s2 | n=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>14:00-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>15:00-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>16:00-17:00</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>taller_2 | agu, joseto | fono:5, kine:7 | s1 | n=2</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>taller_2 | agu, joseto | fono:5, kine:7 | s1 | n=2</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>17:00-18:00</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1393,8 +700,8 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="53" customWidth="1" min="3" max="3"/>
-    <col width="53" customWidth="1" min="4" max="4"/>
+    <col width="37" customWidth="1" min="3" max="3"/>
+    <col width="37" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1410,12 +717,12 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>agu</t>
+          <t>javi</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>joseto</t>
+          <t>maca</t>
         </is>
       </c>
     </row>
@@ -1478,11 +785,6 @@
           <t>12:00-13:00</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>kine_1 | joseto | kine:7 | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1497,7 +799,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -1512,6 +814,11 @@
           <t>15:00-16:00</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1524,11 +831,6 @@
           <t>16:00-17:00</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1541,16 +843,6 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>tea_group | agu, joseto | fono:5, kine:7 | s2 | n=2</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>tea_group | agu, joseto | fono:5, kine:7 | s2 | n=2</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1563,6 +855,11 @@
           <t>08:00-09:00</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1575,11 +872,6 @@
           <t>09:00-10:00</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1592,6 +884,11 @@
           <t>10:00-11:00</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1736,6 +1033,11 @@
           <t>14:00-15:00</t>
         </is>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1772,6 +1074,11 @@
           <t>17:00-18:00</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1784,11 +1091,6 @@
           <t>08:00-09:00</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1861,11 +1163,6 @@
           <t>15:00-16:00</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:7 | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1890,11 +1187,6 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>kine_1 | joseto | kine:7 | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1907,11 +1199,6 @@
           <t>08:00-09:00</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>fono_1 | joseto | fono:5 | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1924,11 +1211,6 @@
           <t>09:00-10:00</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:7 | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1965,11 +1247,6 @@
           <t>12:00-13:00</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:7 | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2006,14 +1283,615 @@
           <t>16:00-17:00</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>taller_2 | agu, joseto | fono:5, kine:7 | s1 | n=2</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>taller_2 | agu, joseto | fono:5, kine:7 | s1 | n=2</t>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="37" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>agu</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>17:00-18:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>08:00-09:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>09:00-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>10:00-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>11:00-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>12:00-13:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>14:00-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>15:00-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>16:00-17:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add bulk select for days and slots in availability grid
Enhanced the AvailabilityGrid component to allow users to select or deselect all slots in a day or all days for a specific slot via header and row buttons. This improves usability for managing large availability schedules. Updated related output files to reflect new availability and schedule data.
</commit_message>
<xml_diff>
--- a/output/schedule.xlsx
+++ b/output/schedule.xlsx
@@ -425,10 +425,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="37" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
     <col width="37" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="37" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -484,11 +484,6 @@
           <t>10:00-11:00</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -496,6 +491,11 @@
           <t>11:00-12:00</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -517,11 +517,6 @@
           <t>15:00-16:00</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -536,7 +531,12 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>kine_1 | agu | kine:javi | s1 | n=1</t>
         </is>
@@ -562,10 +562,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="37" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
     <col width="37" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="37" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -607,11 +607,6 @@
           <t>08:00-09:00</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -640,6 +635,11 @@
           <t>12:00-13:00</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -647,21 +647,21 @@
           <t>14:00-15:00</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
           <t>15:00-16:00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -797,11 +797,6 @@
           <t>14:00-15:00</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -814,11 +809,6 @@
           <t>15:00-16:00</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -855,11 +845,6 @@
           <t>08:00-09:00</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -884,11 +869,6 @@
           <t>10:00-11:00</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -937,6 +917,11 @@
           <t>15:00-16:00</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -961,6 +946,11 @@
           <t>17:00-18:00</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1009,6 +999,11 @@
           <t>11:00-12:00</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1021,6 +1016,11 @@
           <t>12:00-13:00</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1033,11 +1033,6 @@
           <t>14:00-15:00</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1074,11 +1069,6 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1163,6 +1153,11 @@
           <t>15:00-16:00</t>
         </is>
       </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1185,6 +1180,11 @@
       <c r="B37" t="inlineStr">
         <is>
           <t>17:00-18:00</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
         </is>
       </c>
     </row>
@@ -1408,11 +1408,6 @@
           <t>14:00-15:00</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1425,11 +1420,6 @@
           <t>15:00-16:00</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1466,11 +1456,6 @@
           <t>08:00-09:00</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1495,11 +1480,6 @@
           <t>10:00-11:00</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1548,6 +1528,11 @@
           <t>15:00-16:00</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1572,6 +1557,11 @@
           <t>17:00-18:00</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1620,6 +1610,11 @@
           <t>11:00-12:00</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1632,6 +1627,11 @@
           <t>12:00-13:00</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1644,11 +1644,6 @@
           <t>14:00-15:00</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1685,11 +1680,6 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1774,6 +1764,11 @@
           <t>15:00-16:00</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1796,6 +1791,11 @@
       <c r="B37" t="inlineStr">
         <is>
           <t>17:00-18:00</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add API authentication, GCP deploy infra, and UI login
Introduces authentication to the API and UI, including user/session management and JWT-based login. Adds a new Dockerfile for the API, a Terraform-based GCP deployment (Cloud Run, GCS, Artifact Registry), and Makefile targets for cloud deployment and API testing. Updates the README with detailed deployment and usage instructions. Adds new endpoints and logic for user entities, session storage, and Excel download. Updates dependencies and .gitignore for new infra and runtime files.
</commit_message>
<xml_diff>
--- a/output/schedule.xlsx
+++ b/output/schedule.xlsx
@@ -425,10 +425,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="37" customWidth="1" min="2" max="2"/>
     <col width="37" customWidth="1" min="3" max="3"/>
     <col width="37" customWidth="1" min="4" max="4"/>
-    <col width="37" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -491,7 +491,7 @@
           <t>11:00-12:00</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>kine_1 | agu | kine:javi | s1 | n=1</t>
         </is>
@@ -531,12 +531,12 @@
           <t>17:00-18:00</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>kine_1 | agu | kine:javi | s1 | n=1</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>kine_1 | agu | kine:javi | s1 | n=1</t>
         </is>
@@ -562,10 +562,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="37" customWidth="1" min="4" max="4"/>
-    <col width="37" customWidth="1" min="5" max="5"/>
+    <col width="55" customWidth="1" min="2" max="2"/>
+    <col width="55" customWidth="1" min="3" max="3"/>
+    <col width="55" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -614,6 +614,11 @@
           <t>09:00-10:00</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>taller_verano | agu | fono:maca, kine:javi | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -628,6 +633,11 @@
           <t>11:00-12:00</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>taller_verano | agu | fono:maca, kine:javi | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -635,11 +645,6 @@
           <t>12:00-13:00</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -647,6 +652,11 @@
           <t>14:00-15:00</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -659,7 +669,7 @@
           <t>fono_1 | agu | fono:maca | s2 | n=1</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>fono_1 | agu | fono:maca | s2 | n=1</t>
         </is>
@@ -676,6 +686,11 @@
       <c r="A10" t="inlineStr">
         <is>
           <t>17:00-18:00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>taller_verano | agu | fono:maca, kine:javi | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -700,8 +715,8 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="37" customWidth="1" min="4" max="4"/>
+    <col width="55" customWidth="1" min="3" max="3"/>
+    <col width="55" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -749,6 +764,16 @@
           <t>09:00-10:00</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>taller_verano | agu | fono:maca, kine:javi | s2 | n=1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>taller_verano | agu | fono:maca, kine:javi | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -797,6 +822,11 @@
           <t>14:00-15:00</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -833,6 +863,11 @@
           <t>17:00-18:00</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -881,6 +916,11 @@
           <t>11:00-12:00</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -948,7 +988,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+          <t>taller_verano | agu | fono:maca, kine:javi | s2 | n=1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>taller_verano | agu | fono:maca, kine:javi | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1046,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+          <t>taller_verano | agu | fono:maca, kine:javi | s2 | n=1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>taller_verano | agu | fono:maca, kine:javi | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -1016,11 +1066,6 @@
           <t>12:00-13:00</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1045,6 +1090,11 @@
           <t>15:00-16:00</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1069,6 +1119,11 @@
           <t>17:00-18:00</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1153,11 +1208,6 @@
           <t>15:00-16:00</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1180,11 +1230,6 @@
       <c r="B37" t="inlineStr">
         <is>
           <t>17:00-18:00</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1362,7 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="37" customWidth="1" min="3" max="3"/>
+    <col width="55" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1360,6 +1405,11 @@
           <t>09:00-10:00</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>taller_verano | agu | fono:maca, kine:javi | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1408,6 +1458,11 @@
           <t>14:00-15:00</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1444,6 +1499,11 @@
           <t>17:00-18:00</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1492,6 +1552,11 @@
           <t>11:00-12:00</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1559,7 +1624,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+          <t>taller_verano | agu | fono:maca, kine:javi | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -1612,7 +1677,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+          <t>taller_verano | agu | fono:maca, kine:javi | s2 | n=1</t>
         </is>
       </c>
     </row>
@@ -1627,11 +1692,6 @@
           <t>12:00-13:00</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1656,6 +1716,11 @@
           <t>15:00-16:00</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1680,6 +1745,11 @@
           <t>17:00-18:00</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1764,11 +1834,6 @@
           <t>15:00-16:00</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>fono_1 | agu | fono:maca | s2 | n=1</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1791,11 +1856,6 @@
       <c r="B37" t="inlineStr">
         <is>
           <t>17:00-18:00</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>kine_1 | agu | kine:javi | s1 | n=1</t>
         </is>
       </c>
     </row>

</xml_diff>